<commit_message>
based on sagar's comments changes are done
</commit_message>
<xml_diff>
--- a/config/file.xlsx
+++ b/config/file.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="file" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">url</t>
   </si>
@@ -37,7 +38,16 @@
     <t xml:space="preserve">Email-id</t>
   </si>
   <si>
-    <t xml:space="preserve">identity/v1/identity/EMAIL/{email}/details</t>
+    <t xml:space="preserve">Body for success scenarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Body for Negative scenarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v1/otac/email/issue</t>
   </si>
   <si>
     <t xml:space="preserve">harry234@mailinator.com</t>
@@ -51,7 +61,164 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve">{
+  "template": "Your otac {OTC}",
+  "subject": "test",
+  "address": "idtest@mailinator.com",
+  "senderAddress": "idtest@mailinator.com"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v1/otac/phone/issue</t>
+  </si>
+  <si>
     <t xml:space="preserve">harry23@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "template": "{OTAC}",
+  "address": "447789654389",
+  "otacSmsDelay": 0
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "template": "{OTC}",
+  "address": "447789654389",
+  "otacSmsDelay": 0
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v2/otac/email/redeem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "otac": "999999",
+  "address": "idtest@mailinator.com"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "otac": "99999",
+  "address": "idtest@mailinator.com"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v2/otac/phone/redeem</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{
+  "otac": "999999",
+  "address": {
+    "msisdn": "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">447789654389</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"
+  }
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{
+  "otac": "99999",
+  "address": {
+    "msisdn": "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">447789654389</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"
+  }
+}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">v1/message/email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "delivery": {
+        "template": "sms/priority.vm",
+        "subject": "identity test",
+        "address": "idtest153@o2.com",
+        "senderAddress": "idtest153@o2.com"
+    },
+    "tokens": {}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "delivery": {
+        "template": "",
+        "subject": "identity test",
+        "address": "idtest153@o2.com",
+        "senderAddress": "idtest153@o2.com"
+    },
+    "tokens": {}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v1/message/sms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "delivery": {
+    "template": "sms/priority.vm",
+    "address": "+447765432190",
+    "otacSmsDelay": 0
+  },
+  "tokens": {}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "delivery": {
+    "template": "",
+    "address": "+447765432190",
+    "otacSmsDelay": 0
+  },
+  "tokens": {}
+}</t>
   </si>
   <si>
     <t xml:space="preserve">tinyurl/</t>
@@ -65,6 +232,12 @@
   <si>
     <t xml:space="preserve">{
    "duration":"PT2H",
+   "target_url":"http://google.com"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+   "duration":"P1H",
    "target_url":"http://google.com"
 }</t>
   </si>
@@ -76,7 +249,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -97,6 +270,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,12 +319,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -167,18 +353,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="66.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -197,41 +385,106 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>448147724401</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="67.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>448147724431</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="67.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="67.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="67.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="67.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -243,4 +496,27 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>